<commit_message>
add: Julia code for  MPTSPs with subtour elimination
</commit_message>
<xml_diff>
--- a/note/SIPLIB_survey.xlsx
+++ b/note/SIPLIB_survey.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="111">
   <si>
     <t xml:space="preserve">Methods</t>
   </si>
@@ -461,7 +461,7 @@
     <t xml:space="preserve">Source</t>
   </si>
   <si>
-    <t xml:space="preserve">url</t>
+    <t xml:space="preserve">JuMP.Model</t>
   </si>
   <si>
     <t xml:space="preserve">DCAP</t>
@@ -485,22 +485,19 @@
     <t xml:space="preserve">SIPLIB 1.0</t>
   </si>
   <si>
-    <t xml:space="preserve">EXPUTIL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utility Maximization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maximizing a class of submodular utility functions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Math Prog, 2011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MPTSP</t>
+    <t xml:space="preserve">O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPTSPS</t>
   </si>
   <si>
     <t xml:space="preserve">TSP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAR2, GEN1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GEN1</t>
   </si>
   <si>
     <t xml:space="preserve">The multi-path Traveling Salesman Problem with stochastic travel costs</t>
@@ -829,6 +826,10 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -871,10 +872,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -928,7 +925,7 @@
   </sheetPr>
   <dimension ref="A2:G8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -1070,10 +1067,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:AMJ25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1081,260 +1078,251 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="50.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="38.1"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.08"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C1" s="5" t="s">
+    <row r="1" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5" t="s">
+      <c r="D1" s="6"/>
+      <c r="E1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="5"/>
-    </row>
-    <row r="2" s="6" customFormat="true" ht="35.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="F1" s="6"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" s="7" customFormat="true" ht="35.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="7" t="s">
         <v>38</v>
       </c>
+      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8" t="s">
+      <c r="D3" s="9"/>
+      <c r="E3" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="9" t="s">
+      <c r="F3" s="9"/>
+      <c r="G3" s="10" t="s">
         <v>43</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="11" t="s">
         <v>45</v>
       </c>
+      <c r="J3" s="4" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="8" t="s">
+      <c r="A4" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="B4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8" t="s">
+      <c r="D4" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="9" t="s">
-        <v>48</v>
+      <c r="F4" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="I4" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" s="11" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="9" t="s">
-        <v>52</v>
+      <c r="A5" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>56</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="I5" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I5" s="11" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>57</v>
+        <v>42</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>60</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="I6" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="I6" s="11" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>61</v>
+        <v>41</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>64</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="I7" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I7" s="11" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>65</v>
+        <v>68</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="I8" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="I8" s="11" t="s">
         <v>45</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>70</v>
+        <v>72</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>73</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="G10" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H10" s="0" t="s">
+      <c r="I9" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="I10" s="0" t="s">
+      <c r="J9" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N25" s="0" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N26" s="0" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="I3:I9"/>
+    <mergeCell ref="I3:I8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G3" r:id="rId1" display="Dynamic Capacity Acquisition and Assignment under Uncertainty"/>
-    <hyperlink ref="G4" r:id="rId2" display="Maximizing a class of submodular utility functions"/>
-    <hyperlink ref="G5" r:id="rId3" display="The multi-path Traveling Salesman Problem with stochastic travel costs"/>
-    <hyperlink ref="G6" r:id="rId4" display="Robust Capacity Planning in Semiconductor Manufacturing"/>
-    <hyperlink ref="G7" r:id="rId5" display="Improving the integer L-shaped method"/>
-    <hyperlink ref="G8" r:id="rId6" display="Selection of an optimal subset of sizes"/>
-    <hyperlink ref="G9" r:id="rId7" display="The ‘million-variable’ march for stochastic combinatorial optimization"/>
-    <hyperlink ref="G10" r:id="rId8" display="Multiarea Stochastic Unit Commitment for High Wind Penetration in a Transmission Constrained Network"/>
+    <hyperlink ref="G4" r:id="rId2" display="The multi-path Traveling Salesman Problem with stochastic travel costs"/>
+    <hyperlink ref="G5" r:id="rId3" display="Robust Capacity Planning in Semiconductor Manufacturing"/>
+    <hyperlink ref="G6" r:id="rId4" display="Improving the integer L-shaped method"/>
+    <hyperlink ref="G7" r:id="rId5" display="Selection of an optimal subset of sizes"/>
+    <hyperlink ref="G8" r:id="rId6" display="The ‘million-variable’ march for stochastic combinatorial optimization"/>
+    <hyperlink ref="G9" r:id="rId7" display="Multiarea Stochastic Unit Commitment for High Wind Penetration in a Transmission Constrained Network"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1353,51 +1341,51 @@
   </sheetPr>
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="28.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="28.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="47.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="25.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="24.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+    <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14" t="s">
+      <c r="G1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="2" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13"/>
+      <c r="A2" s="14"/>
       <c r="B2" s="16" t="s">
         <v>34</v>
       </c>
@@ -1410,155 +1398,155 @@
       <c r="E2" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
       <c r="F3" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="H3" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="I3" s="19" t="s">
         <v>84</v>
-      </c>
-      <c r="I3" s="19" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" s="19"/>
       <c r="C4" s="19"/>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
       <c r="F4" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="H4" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="I4" s="19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="13" t="s">
         <v>88</v>
-      </c>
-      <c r="I4" s="19" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="s">
-        <v>89</v>
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
       <c r="F5" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="G5" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="H5" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="I5" s="19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="13" t="s">
         <v>92</v>
-      </c>
-      <c r="I5" s="19" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
-        <v>93</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
       <c r="E6" s="19"/>
       <c r="F6" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="G6" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="H6" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="I6" s="19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="I6" s="19" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="s">
+      <c r="F7" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="G7" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="H7" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="I7" s="19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="I7" s="19" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12" t="s">
+      <c r="F8" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="G8" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="H8" s="0" t="s">
         <v>103</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="F9" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="G9" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="G9" s="21" t="s">
+      <c r="H9" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="H9" s="0" t="s">
-        <v>108</v>
-      </c>
       <c r="I9" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" s="22" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F10" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="G10" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="G10" s="23" t="s">
+      <c r="H10" s="22" t="s">
         <v>110</v>
-      </c>
-      <c r="H10" s="22" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add: Multiple Stochastic binary Knapsack Problem (MSKP) julia code
</commit_message>
<xml_diff>
--- a/note/SIPLIB_survey.xlsx
+++ b/note/SIPLIB_survey.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="112">
   <si>
     <t xml:space="preserve">Methods</t>
   </si>
@@ -519,6 +519,9 @@
   </si>
   <si>
     <t xml:space="preserve">Naval Research Logistics, 2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data not available</t>
   </si>
   <si>
     <t xml:space="preserve">SMKP</t>
@@ -1070,7 +1073,7 @@
   <dimension ref="A1:AMJ25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="L10" activeCellId="0" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1085,7 +1088,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.08"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1188,6 +1192,9 @@
       <c r="I4" s="11" t="s">
         <v>45</v>
       </c>
+      <c r="J4" s="4" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -1211,13 +1218,16 @@
       <c r="I5" s="11" t="s">
         <v>45</v>
       </c>
+      <c r="K5" s="0" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>42</v>
@@ -1226,10 +1236,10 @@
         <v>42</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I6" s="11" t="s">
         <v>45</v>
@@ -1237,10 +1247,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>41</v>
@@ -1249,10 +1259,10 @@
         <v>41</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I7" s="11" t="s">
         <v>45</v>
@@ -1260,22 +1270,22 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>42</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I8" s="11" t="s">
         <v>45</v>
@@ -1286,19 +1296,19 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>46</v>
@@ -1306,7 +1316,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N25" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1361,7 +1371,7 @@
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>30</v>
@@ -1372,7 +1382,7 @@
       </c>
       <c r="E1" s="15"/>
       <c r="F1" s="15" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G1" s="15" t="s">
         <v>1</v>
@@ -1381,7 +1391,7 @@
         <v>36</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1405,148 +1415,148 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="17" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
       <c r="F3" s="19" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I3" s="19" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="17" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B4" s="19"/>
       <c r="C4" s="19"/>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
       <c r="F4" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="I4" s="19" t="s">
         <v>85</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="H4" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="I4" s="19" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="13" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
       <c r="F5" s="19" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="13" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
       <c r="E6" s="19"/>
       <c r="F6" s="19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H6" s="19" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I6" s="19" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H7" s="19" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I7" s="19" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G8" s="21" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="17" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G9" s="21" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I9" s="19" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" s="22" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="17" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G10" s="23" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H10" s="22" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add: Introduction part in the manuscript
</commit_message>
<xml_diff>
--- a/note/SIPLIB_survey.xlsx
+++ b/note/SIPLIB_survey.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="114">
   <si>
     <t xml:space="preserve">Methods</t>
   </si>
@@ -530,10 +530,16 @@
     <t xml:space="preserve">multiple knapsack</t>
   </si>
   <si>
+    <t xml:space="preserve">KNA1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Improving the integer L-shaped method</t>
   </si>
   <si>
     <t xml:space="preserve">INFORMS JOC, 2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o</t>
   </si>
   <si>
     <t xml:space="preserve">SIZES</t>
@@ -749,12 +755,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF200"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -812,7 +824,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -859,6 +871,18 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -918,6 +942,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFF200"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -1073,7 +1157,7 @@
   <dimension ref="A1:AMJ25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L10" activeCellId="0" sqref="L10"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1196,29 +1280,30 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="H5" s="12" t="s">
         <v>57</v>
       </c>
       <c r="I5" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="K5" s="0" t="s">
+      <c r="J5" s="14"/>
+      <c r="K5" s="12" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1232,25 +1317,34 @@
       <c r="C6" s="0" t="s">
         <v>42</v>
       </c>
+      <c r="D6" s="0" t="s">
+        <v>61</v>
+      </c>
       <c r="E6" s="0" t="s">
         <v>42</v>
       </c>
+      <c r="F6" s="0" t="s">
+        <v>61</v>
+      </c>
       <c r="G6" s="10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I6" s="11" t="s">
         <v>45</v>
       </c>
+      <c r="J6" s="4" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>41</v>
@@ -1258,11 +1352,11 @@
       <c r="E7" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="12" t="s">
-        <v>65</v>
+      <c r="G7" s="15" t="s">
+        <v>67</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I7" s="11" t="s">
         <v>45</v>
@@ -1270,22 +1364,22 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>42</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I8" s="11" t="s">
         <v>45</v>
@@ -1296,19 +1390,19 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>46</v>
@@ -1316,7 +1410,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N25" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1357,7 +1451,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="28.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="16" width="28.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.64"/>
@@ -1370,193 +1464,193 @@
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="B1" s="15" t="s">
+      <c r="A1" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="G1" s="15" t="s">
+      <c r="E1" s="18"/>
+      <c r="F1" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14"/>
-      <c r="B2" s="16" t="s">
+      <c r="I1" s="18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="17"/>
+      <c r="B2" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="G3" s="20" t="s">
+      <c r="A3" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="G3" s="23" t="s">
         <v>85</v>
       </c>
+      <c r="H3" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="I3" s="22" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="G4" s="20" t="s">
+      <c r="A4" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="I4" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="H4" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="I4" s="19" t="s">
-        <v>85</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="G5" s="20" t="s">
+      <c r="A5" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="I5" s="19" t="s">
-        <v>85</v>
+      <c r="G5" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="G6" s="20" t="s">
+      <c r="A6" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="I6" s="19" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13" t="s">
+      <c r="G6" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="H6" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="I6" s="22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" s="22" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="F7" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="I7" s="19" t="s">
-        <v>85</v>
+      <c r="G7" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="H7" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="I7" s="22" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13" t="s">
-        <v>101</v>
+      <c r="A8" s="16" t="s">
+        <v>103</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="G8" s="21" t="s">
-        <v>103</v>
+        <v>104</v>
+      </c>
+      <c r="G8" s="24" t="s">
+        <v>105</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="17" t="s">
-        <v>105</v>
+      <c r="A9" s="20" t="s">
+        <v>107</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="G9" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="G9" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="I9" s="22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" s="25" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="H9" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="I9" s="19" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" s="22" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="F10" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="G10" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="H10" s="22" t="s">
+      <c r="F10" s="25" t="s">
         <v>111</v>
+      </c>
+      <c r="G10" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="H10" s="25" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add: section 2, section 3
</commit_message>
<xml_diff>
--- a/note/SIPLIB_survey.xlsx
+++ b/note/SIPLIB_survey.xlsx
@@ -1012,7 +1012,7 @@
   </sheetPr>
   <dimension ref="A2:G8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -1156,8 +1156,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H25" activeCellId="0" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1165,10 +1165,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="87.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.08"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="11.52"/>
@@ -1445,7 +1445,7 @@
   </sheetPr>
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
modify: Apply some of Dr. Kim's comments
</commit_message>
<xml_diff>
--- a/note/SIPLIB_survey.xlsx
+++ b/note/SIPLIB_survey.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Algorithms" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Test sets (given)" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="New Test sets Candidates" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Existing LIB" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="126">
   <si>
     <t xml:space="preserve">Methods</t>
   </si>
@@ -687,6 +688,42 @@
   </si>
   <si>
     <t xml:space="preserve">OR, 1992</t>
+  </si>
+  <si>
+    <t xml:space="preserve">airlift scheduling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andy Felt’s library</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ariyawansa and Felt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SLP+MISLP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On a New Collection of Stochastic Linear Programming Test Problems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www4.uwsp.edu/math/afelt/slptestset/download.html</t>
   </si>
 </sst>
 </file>
@@ -824,7 +861,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -930,6 +967,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1156,8 +1197,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H25" activeCellId="0" sqref="H25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1168,7 +1209,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="87.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="87.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.08"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="11.52"/>
@@ -1443,10 +1484,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1479,7 +1520,7 @@
         <v>81</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="H1" s="18" t="s">
         <v>36</v>
@@ -1651,6 +1692,30 @@
       </c>
       <c r="H10" s="25" t="s">
         <v>113</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="G11" s="24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="G12" s="24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="G13" s="24" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1674,6 +1739,77 @@
     <hyperlink ref="G8" r:id="rId6" display="A two-stage stochastic programming model for transportation network protection"/>
     <hyperlink ref="G9" r:id="rId7" display="A Set-Partitioning-Based Model for the Stochastic Vehicle Routing Problem"/>
     <hyperlink ref="G10" r:id="rId8" display="A Vehicle Routing Problem with Stochastic Demand"/>
+    <hyperlink ref="G11" r:id="rId9" display="Andy Felt’s library"/>
+    <hyperlink ref="G12" r:id="rId10" display="Andy Felt’s library"/>
+    <hyperlink ref="G13" r:id="rId11" display="Andy Felt’s library"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.96"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="57.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="49.36"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>2002</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="https://www4.uwsp.edu/math/afelt/slptestset/download.html"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>